<commit_message>
Added calcs for extra noun.
</commit_message>
<xml_diff>
--- a/trunk/Calcs.xlsx
+++ b/trunk/Calcs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="28">
   <si>
     <t>Diceware</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Preposition</t>
+  </si>
+  <si>
+    <t>Normal Double Noun</t>
+  </si>
+  <si>
+    <t>Strong Double Noun</t>
   </si>
 </sst>
 </file>
@@ -448,17 +454,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC56"/>
+  <dimension ref="A1:BC74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="M59" sqref="M59:P77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55" x14ac:dyDescent="0.25">
@@ -2651,15 +2659,15 @@
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B48">
-        <f>B42*B43*B44*B45*B46</f>
+        <f>PRODUCT(B42:B47)</f>
         <v>812514240</v>
       </c>
       <c r="C48">
-        <f>C42*C43*C44*C45*C46</f>
+        <f>PRODUCT(C42:C47)</f>
         <v>176183320320</v>
       </c>
       <c r="D48">
-        <f>D42*D43*D44*D45*D46</f>
+        <f>PRODUCT(D42:D47)</f>
         <v>38080085990400</v>
       </c>
       <c r="G48" t="s">
@@ -2690,7 +2698,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B49">
         <f>LOG(B48, 2)</f>
         <v>29.597817856801026</v>
@@ -2731,7 +2739,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
         <v>18</v>
       </c>
@@ -2760,7 +2768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M51" t="s">
         <v>17</v>
       </c>
@@ -2774,36 +2782,36 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H52">
-        <f>H42*H43*H44*H45*H46*H47*H48*H49*H50</f>
+        <f>PRODUCT(H42:H51)</f>
         <v>3146055137280</v>
       </c>
       <c r="I52">
-        <f>I42*I43*I44*I45*I46*I47*I48*I49*I50</f>
+        <f>PRODUCT(I42:I51)</f>
         <v>4093090897674240</v>
       </c>
       <c r="J52">
-        <f>J42*J43*J44*J45*J46*J47*J48*J49*J50</f>
+        <f>PRODUCT(J42:J51)</f>
         <v>5.3080593463738368E+18</v>
       </c>
       <c r="M52" t="s">
         <v>23</v>
       </c>
       <c r="N52">
-        <f>N44-1</f>
+        <f t="shared" ref="N52:P53" si="62">N44-1</f>
         <v>215</v>
       </c>
       <c r="O52">
-        <f>O44-1</f>
+        <f t="shared" si="62"/>
         <v>1295</v>
       </c>
       <c r="P52">
-        <f>P44-1</f>
+        <f t="shared" si="62"/>
         <v>1295</v>
       </c>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H53">
         <f>LOG(H52, 2)</f>
         <v>41.516681094075615</v>
@@ -2820,33 +2828,33 @@
         <v>18</v>
       </c>
       <c r="N53">
-        <f>N45-1</f>
+        <f t="shared" si="62"/>
         <v>215</v>
       </c>
       <c r="O53">
-        <f>O45-1</f>
+        <f t="shared" si="62"/>
         <v>1295</v>
       </c>
       <c r="P53">
-        <f>P45-1</f>
+        <f t="shared" si="62"/>
         <v>7775</v>
       </c>
     </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N55">
-        <f>N42*N43*N44*N45*N46*N47*N48*N49*N50*N51*N52*N53</f>
+        <f>PRODUCT(N42:N54)</f>
         <v>1.704532673378304E+19</v>
       </c>
       <c r="O55">
-        <f>O42*O43*O44*O45*O46*O47*O48*O49*O50*O51*O52*O53</f>
+        <f>PRODUCT(O42:O54)</f>
         <v>1.3357392835470114E+23</v>
       </c>
       <c r="P55">
-        <f>P42*P43*P44*P45*P46*P47*P48*P49*P50*P51*P52*P53</f>
+        <f>PRODUCT(P42:P54)</f>
         <v>2.8870534784927296E+25</v>
       </c>
     </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N56">
         <f>LOG(N55, 2)</f>
         <v>63.886010056939725</v>
@@ -2858,6 +2866,344 @@
       <c r="P56">
         <f>LOG(P55, 2)</f>
         <v>84.577800203845825</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M59" s="2"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60">
+        <v>9</v>
+      </c>
+      <c r="C60">
+        <v>9</v>
+      </c>
+      <c r="D60">
+        <v>9</v>
+      </c>
+      <c r="G60" t="s">
+        <v>21</v>
+      </c>
+      <c r="H60">
+        <v>2</v>
+      </c>
+      <c r="I60">
+        <v>2</v>
+      </c>
+      <c r="J60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61">
+        <f>6*6*6</f>
+        <v>216</v>
+      </c>
+      <c r="C61">
+        <f>6*6*6*6</f>
+        <v>1296</v>
+      </c>
+      <c r="D61">
+        <v>7776</v>
+      </c>
+      <c r="G61" t="s">
+        <v>17</v>
+      </c>
+      <c r="H61">
+        <v>11</v>
+      </c>
+      <c r="I61">
+        <v>11</v>
+      </c>
+      <c r="J61">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62">
+        <v>11</v>
+      </c>
+      <c r="C62">
+        <v>11</v>
+      </c>
+      <c r="D62">
+        <v>11</v>
+      </c>
+      <c r="G62" t="s">
+        <v>18</v>
+      </c>
+      <c r="H62">
+        <f>6*6*6</f>
+        <v>216</v>
+      </c>
+      <c r="I62">
+        <f>6*6*6*6</f>
+        <v>1296</v>
+      </c>
+      <c r="J62">
+        <f>6*6*6*6*6</f>
+        <v>7776</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63">
+        <f>B61-1</f>
+        <v>215</v>
+      </c>
+      <c r="C63">
+        <f>C61-1</f>
+        <v>1295</v>
+      </c>
+      <c r="D63">
+        <f>D61-1</f>
+        <v>7775</v>
+      </c>
+      <c r="G63" t="s">
+        <v>21</v>
+      </c>
+      <c r="H63">
+        <v>2</v>
+      </c>
+      <c r="I63">
+        <v>2</v>
+      </c>
+      <c r="J63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64">
+        <f>6*6*6</f>
+        <v>216</v>
+      </c>
+      <c r="C64">
+        <f>6*6*6*6</f>
+        <v>1296</v>
+      </c>
+      <c r="D64">
+        <v>7776</v>
+      </c>
+      <c r="G64" t="s">
+        <v>17</v>
+      </c>
+      <c r="H64">
+        <v>11</v>
+      </c>
+      <c r="I64">
+        <v>11</v>
+      </c>
+      <c r="J64">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65">
+        <v>9</v>
+      </c>
+      <c r="C65">
+        <v>9</v>
+      </c>
+      <c r="D65">
+        <v>9</v>
+      </c>
+      <c r="G65" t="s">
+        <v>18</v>
+      </c>
+      <c r="H65">
+        <f>H62-1</f>
+        <v>215</v>
+      </c>
+      <c r="I65">
+        <f>I62-1</f>
+        <v>1295</v>
+      </c>
+      <c r="J65">
+        <f>J62-1</f>
+        <v>7775</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66">
+        <f>B63-1</f>
+        <v>214</v>
+      </c>
+      <c r="C66">
+        <f>C63-1</f>
+        <v>1294</v>
+      </c>
+      <c r="D66">
+        <f>D63-1</f>
+        <v>7774</v>
+      </c>
+      <c r="G66" t="s">
+        <v>19</v>
+      </c>
+      <c r="H66">
+        <f>6*6*6</f>
+        <v>216</v>
+      </c>
+      <c r="I66">
+        <f>6*6*6*6</f>
+        <v>1296</v>
+      </c>
+      <c r="J66">
+        <f>6*6*6*6*6</f>
+        <v>7776</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G67" t="s">
+        <v>22</v>
+      </c>
+      <c r="H67">
+        <v>3</v>
+      </c>
+      <c r="I67">
+        <v>3</v>
+      </c>
+      <c r="J67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <f>PRODUCT(B60:B67)</f>
+        <v>1912658520960</v>
+      </c>
+      <c r="C68">
+        <f>PRODUCT(C60:C67)</f>
+        <v>2507793381434880</v>
+      </c>
+      <c r="D68">
+        <f>PRODUCT(D60:D67)</f>
+        <v>3.2563804733830656E+18</v>
+      </c>
+      <c r="G68" t="s">
+        <v>21</v>
+      </c>
+      <c r="H68">
+        <v>2</v>
+      </c>
+      <c r="I68">
+        <v>2</v>
+      </c>
+      <c r="J68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <f>LOG(B68, 2)</f>
+        <v>40.798716461839469</v>
+      </c>
+      <c r="C69">
+        <f>LOG(C68, 2)</f>
+        <v>51.155339911857595</v>
+      </c>
+      <c r="D69">
+        <f>LOG(D68, 2)</f>
+        <v>61.497974980978007</v>
+      </c>
+      <c r="G69" t="s">
+        <v>17</v>
+      </c>
+      <c r="H69">
+        <v>11</v>
+      </c>
+      <c r="I69">
+        <v>11</v>
+      </c>
+      <c r="J69">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G70" t="s">
+        <v>23</v>
+      </c>
+      <c r="H70">
+        <f>6*6*6</f>
+        <v>216</v>
+      </c>
+      <c r="I70">
+        <f>6*6*6*6</f>
+        <v>1296</v>
+      </c>
+      <c r="J70">
+        <f>6*6*6*6*6</f>
+        <v>7776</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G71" t="s">
+        <v>18</v>
+      </c>
+      <c r="H71">
+        <f>H65-1</f>
+        <v>214</v>
+      </c>
+      <c r="I71">
+        <f>I65-1</f>
+        <v>1294</v>
+      </c>
+      <c r="J71">
+        <f>J65-1</f>
+        <v>7774</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H73">
+        <f>PRODUCT(H60:H71)</f>
+        <v>1.481162758631424E+16</v>
+      </c>
+      <c r="I73">
+        <f>PRODUCT(I60:I71)</f>
+        <v>1.1652211167499026E+20</v>
+      </c>
+      <c r="J73">
+        <f>PRODUCT(J60:J71)</f>
+        <v>9.0782677389162453E+23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H74">
+        <f>LOG(H73, 2)</f>
+        <v>53.717579699114061</v>
+      </c>
+      <c r="I74">
+        <f>LOG(I73, 2)</f>
+        <v>66.65916564985335</v>
+      </c>
+      <c r="J74">
+        <f>LOG(J73, 2)</f>
+        <v>79.586763219694916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>